<commit_message>
Initial USB C revision
</commit_message>
<xml_diff>
--- a/Production/BOMs/Makerfabs/3DProUsb-Makerfabs-BOM-DigiKey.xlsx
+++ b/Production/BOMs/Makerfabs/3DProUsb-Makerfabs-BOM-DigiKey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kreeblah/SidewinderToUSBV2/Production/BOMs/Makerfabs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853D6150-E53B-0F4E-822A-6591BB721FA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B894B937-E122-6D4C-A331-A0D5C5E4531F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="760" windowWidth="28040" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3DProUsb-Makerfabs-BOM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="120">
   <si>
     <t>Item #</t>
   </si>
@@ -58,9 +58,6 @@
     <t>J1</t>
   </si>
   <si>
-    <t>CONN RCPT USB2.0 MICRO B SMD R/A</t>
-  </si>
-  <si>
     <t>SMD</t>
   </si>
   <si>
@@ -352,23 +349,44 @@
     <t>C1,C2,C11</t>
   </si>
   <si>
-    <t>Amphenol ICC (FCI)</t>
-  </si>
-  <si>
-    <t>10118193-0001LF</t>
-  </si>
-  <si>
-    <t>DigiKey Part: 609-4616-2-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/products/en?keywords=609-4616-2-ND</t>
+    <t>GCT</t>
+  </si>
+  <si>
+    <t>USB4105-GF-A</t>
+  </si>
+  <si>
+    <t>CONN RCP USB2.0 TYP C 24P SMD RA</t>
+  </si>
+  <si>
+    <t>DigiKey Part: 2073-USB4105-GF-ADKR-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/gct/USB4105-GF-A/11198441</t>
+  </si>
+  <si>
+    <t>R8,R9</t>
+  </si>
+  <si>
+    <t>Panasonic Electronic Components</t>
+  </si>
+  <si>
+    <t>ERA-2APB512X</t>
+  </si>
+  <si>
+    <t>RES SMD 5.1K OHM 0.1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>DigiKey Part: P5.1KCNDKR-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/panasonic-electronic-components/era-2apb512x/5140865</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -693,7 +711,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -823,6 +841,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -869,13 +900,15 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="42" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1232,13 +1265,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
@@ -1249,11 +1282,11 @@
     <col min="7" max="7" width="17" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="35.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="67.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="89" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1285,7 +1318,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -1296,19 +1329,19 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>112</v>
@@ -1317,452 +1350,481 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="C4" s="4">
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="5" t="s">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="5" t="s">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="4" t="s">
+      <c r="J6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J6" s="5" t="s">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="4" t="s">
+      <c r="J7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J7" s="5" t="s">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="J8" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>57</v>
+      <c r="H9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="J9" s="5" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="C10" s="4">
         <v>4</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="4" t="s">
+      <c r="J10" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="J10" s="5" t="s">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="C11" s="4">
         <v>2</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="4" t="s">
+      <c r="J11" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="5" t="s">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="C12" s="4">
         <v>2</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="4" t="s">
+      <c r="J12" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="J12" s="5" t="s">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="C13" s="4">
         <v>2</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="4" t="s">
+      <c r="J13" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="J13" s="5" t="s">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="C14" s="4">
         <v>2</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="4" t="s">
+      <c r="J14" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="J14" s="5" t="s">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="C15" s="4">
         <v>2</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E15" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" s="4" t="s">
+      <c r="J15" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="J15" s="5" t="s">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>100</v>
       </c>
+      <c r="B16" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="6">
+        <v>1</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="G16" s="6">
+        <v>1206</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>105</v>
+      </c>
     </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C16" s="4">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G16" s="4">
-        <v>1206</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>106</v>
+    <row r="17" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1781,6 +1843,7 @@
     <hyperlink ref="J8" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="J9" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="J10" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="J17" r:id="rId15" xr:uid="{5490E745-1773-0E46-B7D1-DD0C1E68025C}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>